<commit_message>
feat: adição de e-mail do cliente no arquivo da Estante Virtual
</commit_message>
<xml_diff>
--- a/public/upload-file/template/Envio de pedidos Estante Virtual.xlsx
+++ b/public/upload-file/template/Envio de pedidos Estante Virtual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LowCost\Projetos\B1Sistema-PDOCRUD\resources\react-app\public\upload-file\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1665DD3D-F7A6-484B-BC60-9811181F12D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7BE763-0AC5-4346-AAA3-03359335845B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="1710" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Data de pagamento</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>Data para envio</t>
+  </si>
+  <si>
+    <t>E-mail do Comprador</t>
   </si>
 </sst>
 </file>
@@ -495,7 +498,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF2"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -503,11 +506,11 @@
   <cols>
     <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.7265625" customWidth="1"/>
+    <col min="31" max="31" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,73 +545,76 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="AD2" s="1"/>
       <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: correção na exportação de planilha da Estante Virtual para o Bling
</commit_message>
<xml_diff>
--- a/public/upload-file/template/Envio de pedidos Estante Virtual.xlsx
+++ b/public/upload-file/template/Envio de pedidos Estante Virtual.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LowCost\Projetos\B1Sistema-PDOCRUD\resources\react-app\public\upload-file\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7BE763-0AC5-4346-AAA3-03359335845B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F48342B-5B5C-44B2-9F5D-B5FF44715624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="1710" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Data de pagamento</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>E-mail do Comprador</t>
+  </si>
+  <si>
+    <t>Nº Checkout</t>
   </si>
 </sst>
 </file>
@@ -178,9 +181,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -218,9 +221,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -253,26 +256,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -305,26 +291,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -498,7 +467,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -506,11 +475,12 @@
   <cols>
     <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -518,34 +488,34 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>32</v>
       </c>
       <c r="M1" t="s">
         <v>11</v>
@@ -610,8 +580,11 @@
       <c r="AG1" t="s">
         <v>30</v>
       </c>
+      <c r="AH1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>

</xml_diff>